<commit_message>
Diseñados casos de prueba StackWeapon
Solucionado implementación del StackWeapon
</commit_message>
<xml_diff>
--- a/Bibliografía/BD Armas.xlsx
+++ b/Bibliografía/BD Armas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDLABU2\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7109D3B-32E2-4B3F-8B01-468028847CB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7E0000-C279-45E9-B0B4-433E4A96164D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{03C55EC9-E2CB-4149-9FAD-4D29EBE966AF}"/>
   </bookViews>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B14604-B078-4631-A77D-F39DE93A486B}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection sqref="A1:D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>